<commit_message>
adding budget justification v.1
</commit_message>
<xml_diff>
--- a/Shrimpton-NSF-Small-budget-V3.xlsx
+++ b/Shrimpton-NSF-Small-budget-V3.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="500" yWindow="8320" windowWidth="25840" windowHeight="16920"/>
+    <workbookView xWindow="-52900" yWindow="11060" windowWidth="25840" windowHeight="16920"/>
   </bookViews>
   <sheets>
     <sheet name="Shrimpton" sheetId="1" r:id="rId1"/>
@@ -1225,8 +1225,8 @@
   </sheetPr>
   <dimension ref="A1:AD62"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -1411,18 +1411,18 @@
         <v>28982</v>
       </c>
       <c r="F6" s="26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6" s="23">
         <f>ROUND(W6/X6*F6,0)</f>
-        <v>29852</v>
+        <v>14926</v>
       </c>
       <c r="H6" s="26">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="I6" s="23">
         <f>ROUND(Y6/Z6*H6,0)</f>
-        <v>23060</v>
+        <v>15374</v>
       </c>
       <c r="J6" s="26">
         <v>0</v>
@@ -1440,12 +1440,12 @@
       </c>
       <c r="N6" s="24">
         <f>M6+K6+I6+G6+E6</f>
-        <v>81894</v>
+        <v>59282</v>
       </c>
       <c r="O6" s="72"/>
       <c r="P6" s="73">
         <f>N6+O6</f>
-        <v>81894</v>
+        <v>59282</v>
       </c>
       <c r="Q6" s="4"/>
       <c r="R6" s="1" t="s">
@@ -1581,12 +1581,12 @@
       <c r="F11" s="4"/>
       <c r="G11" s="24">
         <f>SUM(G6:G10)</f>
-        <v>29852</v>
+        <v>14926</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="24">
         <f>SUM(I6:I10)</f>
-        <v>23060</v>
+        <v>15374</v>
       </c>
       <c r="J11" s="4"/>
       <c r="K11" s="24">
@@ -1600,12 +1600,12 @@
       </c>
       <c r="N11" s="24">
         <f t="shared" ref="N11:N47" si="0">M11+K11+I11+G11+E11</f>
-        <v>81894</v>
+        <v>59282</v>
       </c>
       <c r="O11" s="72"/>
       <c r="P11" s="73">
         <f>P6</f>
-        <v>81894</v>
+        <v>59282</v>
       </c>
       <c r="Q11" s="4"/>
       <c r="R11" s="1"/>
@@ -1742,11 +1742,11 @@
         <v>51500</v>
       </c>
       <c r="H15" s="26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I15" s="23">
         <f>ROUND((C15*1.03^2)*H15,0)</f>
-        <v>26523</v>
+        <v>53045</v>
       </c>
       <c r="J15" s="26">
         <v>0</v>
@@ -1764,12 +1764,12 @@
       </c>
       <c r="N15" s="24">
         <f t="shared" si="0"/>
-        <v>128023</v>
+        <v>154545</v>
       </c>
       <c r="O15" s="72"/>
       <c r="P15" s="73">
         <f t="shared" ref="P15:P18" si="1">O15+N15</f>
-        <v>128023</v>
+        <v>154545</v>
       </c>
       <c r="Q15" s="4"/>
       <c r="R15" s="1"/>
@@ -1958,7 +1958,7 @@
       <c r="H19" s="4"/>
       <c r="I19" s="24">
         <f>SUM(I14:I18)</f>
-        <v>26523</v>
+        <v>53045</v>
       </c>
       <c r="J19" s="4"/>
       <c r="K19" s="24">
@@ -1972,12 +1972,12 @@
       </c>
       <c r="N19" s="24">
         <f t="shared" si="0"/>
-        <v>128023</v>
+        <v>154545</v>
       </c>
       <c r="O19" s="72"/>
       <c r="P19" s="73">
         <f>SUM(P14:P18)</f>
-        <v>128023</v>
+        <v>154545</v>
       </c>
       <c r="Q19" s="4"/>
       <c r="R19" s="1"/>
@@ -1996,12 +1996,12 @@
       <c r="F20" s="4"/>
       <c r="G20" s="24">
         <f>G19+G11</f>
-        <v>81352</v>
+        <v>66426</v>
       </c>
       <c r="H20" s="4"/>
       <c r="I20" s="24">
         <f>I19+I11</f>
-        <v>49583</v>
+        <v>68419</v>
       </c>
       <c r="J20" s="4"/>
       <c r="K20" s="24">
@@ -2015,12 +2015,12 @@
       </c>
       <c r="N20" s="24">
         <f t="shared" si="0"/>
-        <v>209917</v>
+        <v>213827</v>
       </c>
       <c r="O20" s="72"/>
       <c r="P20" s="73">
         <f>P19+P11</f>
-        <v>209917</v>
+        <v>213827</v>
       </c>
       <c r="Q20" s="4"/>
       <c r="R20" s="1"/>
@@ -2083,12 +2083,12 @@
       <c r="F23" s="9"/>
       <c r="G23" s="23">
         <f>ROUND(G11*C23,0)</f>
-        <v>8179</v>
+        <v>4090</v>
       </c>
       <c r="H23" s="9"/>
       <c r="I23" s="23">
         <f>ROUND(I11*C23,0)</f>
-        <v>6318</v>
+        <v>4212</v>
       </c>
       <c r="J23" s="9"/>
       <c r="K23" s="23">
@@ -2102,12 +2102,12 @@
       </c>
       <c r="N23" s="24">
         <f t="shared" si="0"/>
-        <v>22438</v>
+        <v>16243</v>
       </c>
       <c r="O23" s="72"/>
       <c r="P23" s="73">
         <f>O23+N23</f>
-        <v>22438</v>
+        <v>16243</v>
       </c>
       <c r="Q23" s="4"/>
       <c r="R23" s="1"/>
@@ -2178,7 +2178,7 @@
       <c r="H25" s="9"/>
       <c r="I25" s="23">
         <f>ROUND(I15*C25,0)</f>
-        <v>2705</v>
+        <v>5411</v>
       </c>
       <c r="J25" s="9"/>
       <c r="K25" s="23">
@@ -2192,12 +2192,12 @@
       </c>
       <c r="N25" s="24">
         <f t="shared" si="0"/>
-        <v>13058</v>
+        <v>15764</v>
       </c>
       <c r="O25" s="72"/>
       <c r="P25" s="73">
         <f t="shared" si="4"/>
-        <v>13058</v>
+        <v>15764</v>
       </c>
       <c r="Q25" s="4"/>
       <c r="R25" s="1"/>
@@ -2351,12 +2351,12 @@
       <c r="F29" s="4"/>
       <c r="G29" s="24">
         <f>SUM(G23:G28)</f>
-        <v>13432</v>
+        <v>9343</v>
       </c>
       <c r="H29" s="4"/>
       <c r="I29" s="24">
         <f>SUM(I23:I28)</f>
-        <v>9023</v>
+        <v>9623</v>
       </c>
       <c r="J29" s="4"/>
       <c r="K29" s="24">
@@ -2370,12 +2370,12 @@
       </c>
       <c r="N29" s="24">
         <f t="shared" si="0"/>
-        <v>35496</v>
+        <v>32007</v>
       </c>
       <c r="O29" s="72"/>
       <c r="P29" s="73">
         <f>SUM(P23:P28)</f>
-        <v>35496</v>
+        <v>32007</v>
       </c>
       <c r="Q29" s="4"/>
       <c r="R29" s="1"/>
@@ -2394,12 +2394,12 @@
       <c r="F30" s="4"/>
       <c r="G30" s="24">
         <f>G29+G20</f>
-        <v>94784</v>
+        <v>75769</v>
       </c>
       <c r="H30" s="4"/>
       <c r="I30" s="24">
         <f>I29+I20</f>
-        <v>58606</v>
+        <v>78042</v>
       </c>
       <c r="J30" s="4"/>
       <c r="K30" s="24">
@@ -2413,12 +2413,12 @@
       </c>
       <c r="N30" s="24">
         <f t="shared" si="0"/>
-        <v>245413</v>
+        <v>245834</v>
       </c>
       <c r="O30" s="72"/>
       <c r="P30" s="73">
         <f>P29+P20</f>
-        <v>245413</v>
+        <v>245834</v>
       </c>
       <c r="Q30" s="4"/>
       <c r="R30" s="1"/>
@@ -2775,7 +2775,7 @@
       <c r="H41" s="27"/>
       <c r="I41" s="23">
         <f>ROUND((A59*1.05^2)*H15,0)</f>
-        <v>12467</v>
+        <v>24934</v>
       </c>
       <c r="J41" s="27"/>
       <c r="K41" s="23">
@@ -2789,12 +2789,12 @@
       </c>
       <c r="N41" s="24">
         <f t="shared" si="0"/>
-        <v>58830</v>
+        <v>71297</v>
       </c>
       <c r="O41" s="72"/>
       <c r="P41" s="73">
         <f>O41+N41</f>
-        <v>58830</v>
+        <v>71297</v>
       </c>
       <c r="Q41" s="4"/>
       <c r="R41" s="1"/>
@@ -3010,7 +3010,7 @@
       <c r="H47" s="4"/>
       <c r="I47" s="24">
         <f>SUM(I41:I46)</f>
-        <v>12467</v>
+        <v>24934</v>
       </c>
       <c r="J47" s="4"/>
       <c r="K47" s="24">
@@ -3024,12 +3024,12 @@
       </c>
       <c r="N47" s="24">
         <f t="shared" si="0"/>
-        <v>58830</v>
+        <v>71297</v>
       </c>
       <c r="O47" s="72"/>
       <c r="P47" s="73">
         <f>SUM(P41:P46)</f>
-        <v>58830</v>
+        <v>71297</v>
       </c>
       <c r="Q47" s="4"/>
       <c r="R47" s="1"/>
@@ -3068,12 +3068,12 @@
       <c r="F49" s="4"/>
       <c r="G49" s="24">
         <f>G47+G39+G30</f>
-        <v>129531</v>
+        <v>110516</v>
       </c>
       <c r="H49" s="4"/>
       <c r="I49" s="24">
         <f>I47+I39+I30</f>
-        <v>82073</v>
+        <v>113976</v>
       </c>
       <c r="J49" s="4"/>
       <c r="K49" s="24">
@@ -3087,12 +3087,12 @@
       </c>
       <c r="N49" s="24">
         <f>M49+K49+I49+G49+E49</f>
-        <v>337243</v>
+        <v>350131</v>
       </c>
       <c r="O49" s="72"/>
       <c r="P49" s="73">
         <f>P47+P39+P30</f>
-        <v>337243</v>
+        <v>350131</v>
       </c>
       <c r="Q49" s="4"/>
       <c r="R49" s="1"/>
@@ -3111,12 +3111,12 @@
       <c r="F50" s="69"/>
       <c r="G50" s="69">
         <f t="shared" ref="G50:M50" si="11">G49-G47</f>
-        <v>105784</v>
+        <v>86769</v>
       </c>
       <c r="H50" s="69"/>
       <c r="I50" s="69">
         <f t="shared" si="11"/>
-        <v>69606</v>
+        <v>89042</v>
       </c>
       <c r="J50" s="69"/>
       <c r="K50" s="69">
@@ -3130,12 +3130,12 @@
       </c>
       <c r="N50" s="69">
         <f>M50+K50+I50+G50+E50</f>
-        <v>278413</v>
+        <v>278834</v>
       </c>
       <c r="O50" s="72"/>
       <c r="P50" s="73">
         <f>P49-P47</f>
-        <v>278413</v>
+        <v>278834</v>
       </c>
       <c r="Q50" s="4"/>
       <c r="R50" s="1"/>
@@ -3163,12 +3163,12 @@
       <c r="F52" s="4"/>
       <c r="G52" s="47">
         <f>ROUND((G49-G47)*C52,0)</f>
-        <v>55537</v>
+        <v>45554</v>
       </c>
       <c r="H52" s="4"/>
       <c r="I52" s="24">
         <f>ROUND((I49-I47)*C52,0)</f>
-        <v>36543</v>
+        <v>46747</v>
       </c>
       <c r="J52" s="4"/>
       <c r="K52" s="24">
@@ -3182,12 +3182,12 @@
       </c>
       <c r="N52" s="24">
         <f>M52+K52+I52+G52+E52</f>
-        <v>146167</v>
+        <v>146388</v>
       </c>
       <c r="O52" s="72"/>
       <c r="P52" s="73">
         <f>O52+N52</f>
-        <v>146167</v>
+        <v>146388</v>
       </c>
       <c r="Q52" s="4"/>
       <c r="R52" s="1"/>
@@ -3225,12 +3225,12 @@
       <c r="F54" s="9"/>
       <c r="G54" s="24">
         <f>G52+G49</f>
-        <v>185068</v>
+        <v>156070</v>
       </c>
       <c r="H54" s="9"/>
       <c r="I54" s="24">
         <f>I52+I49</f>
-        <v>118616</v>
+        <v>160723</v>
       </c>
       <c r="J54" s="9"/>
       <c r="K54" s="24">
@@ -3244,12 +3244,12 @@
       </c>
       <c r="N54" s="24">
         <f t="shared" ref="N54" si="12">M54+K54+I54+G54+E54</f>
-        <v>483410</v>
+        <v>496519</v>
       </c>
       <c r="O54" s="75"/>
       <c r="P54" s="76">
         <f>P52+P49</f>
-        <v>483410</v>
+        <v>496519</v>
       </c>
     </row>
     <row r="55" spans="1:18" ht="17" x14ac:dyDescent="0.25">
@@ -15979,19 +15979,19 @@
       </c>
       <c r="F6" s="44">
         <f>Shrimpton!F6</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6" s="46">
         <f>Shrimpton!G6</f>
-        <v>29852</v>
+        <v>14926</v>
       </c>
       <c r="H6" s="44">
         <f>Shrimpton!H6</f>
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="I6" s="46">
         <f>Shrimpton!I6</f>
-        <v>23060</v>
+        <v>15374</v>
       </c>
       <c r="J6" s="44">
         <f>Shrimpton!J6</f>
@@ -16011,7 +16011,7 @@
       </c>
       <c r="N6" s="24">
         <f>M6+K6+I6+G6+E6</f>
-        <v>81894</v>
+        <v>59282</v>
       </c>
       <c r="O6" s="1"/>
       <c r="P6" s="82">
@@ -16024,19 +16024,19 @@
       </c>
       <c r="R6" s="82">
         <f>+F6*0.01</f>
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="S6" s="83">
         <f>+F6*0.99</f>
-        <v>1.98</v>
+        <v>0.99</v>
       </c>
       <c r="T6" s="82">
         <f>+H6*0.01</f>
-        <v>1.4999999999999999E-2</v>
+        <v>0.01</v>
       </c>
       <c r="U6" s="83">
         <f>+H6*0.99</f>
-        <v>1.4849999999999999</v>
+        <v>0.99</v>
       </c>
       <c r="V6" s="82">
         <f>+J6*0.01</f>
@@ -16627,12 +16627,12 @@
       <c r="F13" s="52"/>
       <c r="G13" s="47">
         <f>SUM(G6:G12)</f>
-        <v>29852</v>
+        <v>14926</v>
       </c>
       <c r="H13" s="52"/>
       <c r="I13" s="47">
         <f>SUM(I6:I12)</f>
-        <v>23060</v>
+        <v>15374</v>
       </c>
       <c r="J13" s="52"/>
       <c r="K13" s="47">
@@ -16646,7 +16646,7 @@
       </c>
       <c r="N13" s="24">
         <f t="shared" ref="N13:N51" si="11">M13+K13+I13+G13+E13</f>
-        <v>81894</v>
+        <v>59282</v>
       </c>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
@@ -16790,11 +16790,11 @@
       </c>
       <c r="H17" s="44">
         <f>Shrimpton!H15+'PI 2'!H15+'PI 3'!H15+'PI 4'!H15+'PI 5'!H15+'PI 6'!H15+'PI 7'!H15</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I17" s="44">
         <f>Shrimpton!I15+'PI 2'!I15+'PI 3'!I15+'PI 4'!I15+'PI 5'!I15+'PI 6'!I15+'PI 7'!I15</f>
-        <v>26523</v>
+        <v>53045</v>
       </c>
       <c r="J17" s="44">
         <f>Shrimpton!J15+'PI 2'!J15+'PI 3'!J15+'PI 4'!J15+'PI 5'!J15+'PI 6'!J15+'PI 7'!J15</f>
@@ -16814,7 +16814,7 @@
       </c>
       <c r="N17" s="24">
         <f t="shared" si="11"/>
-        <v>128023</v>
+        <v>154545</v>
       </c>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
@@ -17011,7 +17011,7 @@
       <c r="H21" s="52"/>
       <c r="I21" s="47">
         <f>SUM(I16:I20)</f>
-        <v>26523</v>
+        <v>53045</v>
       </c>
       <c r="J21" s="52"/>
       <c r="K21" s="47">
@@ -17025,7 +17025,7 @@
       </c>
       <c r="N21" s="24">
         <f t="shared" si="11"/>
-        <v>128023</v>
+        <v>154545</v>
       </c>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
@@ -17046,12 +17046,12 @@
       <c r="F22" s="52"/>
       <c r="G22" s="47">
         <f>G21+G13</f>
-        <v>81352</v>
+        <v>66426</v>
       </c>
       <c r="H22" s="52"/>
       <c r="I22" s="47">
         <f>I21+I13</f>
-        <v>49583</v>
+        <v>68419</v>
       </c>
       <c r="J22" s="52"/>
       <c r="K22" s="47">
@@ -17065,7 +17065,7 @@
       </c>
       <c r="N22" s="24">
         <f t="shared" si="11"/>
-        <v>209917</v>
+        <v>213827</v>
       </c>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
@@ -17130,12 +17130,12 @@
       <c r="F25" s="46"/>
       <c r="G25" s="46">
         <f>Shrimpton!G23+'PI 2'!G23+'PI 3'!G23+'PI 4'!G23+'PI 5'!G23+'PI 6'!G23+'PI 7'!G23</f>
-        <v>8179</v>
+        <v>4090</v>
       </c>
       <c r="H25" s="46"/>
       <c r="I25" s="46">
         <f>Shrimpton!I23+'PI 2'!I23+'PI 3'!I23+'PI 4'!I23+'PI 5'!I23+'PI 6'!I23+'PI 7'!I23</f>
-        <v>6318</v>
+        <v>4212</v>
       </c>
       <c r="J25" s="46"/>
       <c r="K25" s="46">
@@ -17149,7 +17149,7 @@
       </c>
       <c r="N25" s="24">
         <f t="shared" si="11"/>
-        <v>22438</v>
+        <v>16243</v>
       </c>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
@@ -17219,7 +17219,7 @@
       <c r="H27" s="46"/>
       <c r="I27" s="46">
         <f>Shrimpton!I25+'PI 2'!I25+'PI 3'!I25+'PI 4'!I25+'PI 5'!I25+'PI 6'!I25+'PI 7'!I25</f>
-        <v>2705</v>
+        <v>5411</v>
       </c>
       <c r="J27" s="46"/>
       <c r="K27" s="46">
@@ -17233,7 +17233,7 @@
       </c>
       <c r="N27" s="24">
         <f t="shared" si="11"/>
-        <v>13058</v>
+        <v>15764</v>
       </c>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
@@ -17380,12 +17380,12 @@
       <c r="F31" s="52"/>
       <c r="G31" s="47">
         <f>SUM(G25:G30)</f>
-        <v>13432</v>
+        <v>9343</v>
       </c>
       <c r="H31" s="52"/>
       <c r="I31" s="47">
         <f>SUM(I25:I30)</f>
-        <v>9023</v>
+        <v>9623</v>
       </c>
       <c r="J31" s="52"/>
       <c r="K31" s="47">
@@ -17399,7 +17399,7 @@
       </c>
       <c r="N31" s="24">
         <f t="shared" si="11"/>
-        <v>35496</v>
+        <v>32007</v>
       </c>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
@@ -17420,12 +17420,12 @@
       <c r="F32" s="52"/>
       <c r="G32" s="47">
         <f>G31+G22</f>
-        <v>94784</v>
+        <v>75769</v>
       </c>
       <c r="H32" s="52"/>
       <c r="I32" s="47">
         <f>I31+I22</f>
-        <v>58606</v>
+        <v>78042</v>
       </c>
       <c r="J32" s="52"/>
       <c r="K32" s="47">
@@ -17439,7 +17439,7 @@
       </c>
       <c r="N32" s="24">
         <f t="shared" si="11"/>
-        <v>245413</v>
+        <v>245834</v>
       </c>
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
@@ -17807,7 +17807,7 @@
       <c r="H43" s="55"/>
       <c r="I43" s="46">
         <f>Shrimpton!I41+'PI 2'!I41+'PI 3'!I41+'PI 4'!I41+'PI 5'!I41+'PI 6'!I41+'PI 7'!I41</f>
-        <v>12467</v>
+        <v>24934</v>
       </c>
       <c r="J43" s="55"/>
       <c r="K43" s="46">
@@ -17821,7 +17821,7 @@
       </c>
       <c r="N43" s="24">
         <f t="shared" si="11"/>
-        <v>58830</v>
+        <v>71297</v>
       </c>
       <c r="O43" s="1"/>
       <c r="P43" s="1"/>
@@ -18049,7 +18049,7 @@
       <c r="H49" s="52"/>
       <c r="I49" s="47">
         <f>SUM(I43:I48)</f>
-        <v>12467</v>
+        <v>24934</v>
       </c>
       <c r="J49" s="52"/>
       <c r="K49" s="47">
@@ -18063,7 +18063,7 @@
       </c>
       <c r="N49" s="24">
         <f t="shared" si="11"/>
-        <v>58830</v>
+        <v>71297</v>
       </c>
       <c r="O49" s="1"/>
       <c r="P49" s="1"/>
@@ -18104,12 +18104,12 @@
       <c r="F51" s="52"/>
       <c r="G51" s="47">
         <f>G49+G41+G32</f>
-        <v>129531</v>
+        <v>110516</v>
       </c>
       <c r="H51" s="52"/>
       <c r="I51" s="47">
         <f>I49+I41+I32</f>
-        <v>82073</v>
+        <v>113976</v>
       </c>
       <c r="J51" s="52"/>
       <c r="K51" s="47">
@@ -18123,7 +18123,7 @@
       </c>
       <c r="N51" s="24">
         <f t="shared" si="11"/>
-        <v>337243</v>
+        <v>350131</v>
       </c>
       <c r="O51" s="1"/>
       <c r="P51" s="1"/>
@@ -18144,12 +18144,12 @@
       <c r="F52" s="69"/>
       <c r="G52" s="69">
         <f t="shared" ref="G52:M52" si="12">G51-G49</f>
-        <v>105784</v>
+        <v>86769</v>
       </c>
       <c r="H52" s="69"/>
       <c r="I52" s="69">
         <f t="shared" si="12"/>
-        <v>69606</v>
+        <v>89042</v>
       </c>
       <c r="J52" s="69"/>
       <c r="K52" s="69">
@@ -18163,7 +18163,7 @@
       </c>
       <c r="N52" s="69">
         <f>M52+K52+I52+G52+E52</f>
-        <v>278413</v>
+        <v>278834</v>
       </c>
       <c r="O52" s="1"/>
       <c r="P52" s="1"/>
@@ -18193,12 +18193,12 @@
       <c r="F54" s="52"/>
       <c r="G54" s="47">
         <f>Shrimpton!G52+'PI 2'!G52+'PI 3'!G52+'PI 4'!G52+'PI 5'!G52+'PI 6'!G52+'PI 7'!G52</f>
-        <v>55537</v>
+        <v>45554</v>
       </c>
       <c r="H54" s="52"/>
       <c r="I54" s="47">
         <f>Shrimpton!I52+'PI 2'!I52+'PI 3'!I52+'PI 4'!I52+'PI 5'!I52+'PI 6'!I52+'PI 7'!I52</f>
-        <v>36543</v>
+        <v>46747</v>
       </c>
       <c r="J54" s="52"/>
       <c r="K54" s="47">
@@ -18212,7 +18212,7 @@
       </c>
       <c r="N54" s="24">
         <f>M54+K54+I54+G54+E54</f>
-        <v>146167</v>
+        <v>146388</v>
       </c>
       <c r="O54" s="1"/>
       <c r="P54" s="1"/>
@@ -18252,12 +18252,12 @@
       <c r="F56" s="44"/>
       <c r="G56" s="47">
         <f>G51+G54</f>
-        <v>185068</v>
+        <v>156070</v>
       </c>
       <c r="H56" s="44"/>
       <c r="I56" s="47">
         <f>I54+I51</f>
-        <v>118616</v>
+        <v>160723</v>
       </c>
       <c r="J56" s="44"/>
       <c r="K56" s="47">
@@ -18271,7 +18271,7 @@
       </c>
       <c r="N56" s="24">
         <f>M56+K56+I56+G56+E56</f>
-        <v>483410</v>
+        <v>496519</v>
       </c>
     </row>
     <row r="57" spans="1:18" ht="17" x14ac:dyDescent="0.25">
@@ -18327,7 +18327,7 @@
       <c r="M59"/>
       <c r="N59" s="92">
         <f>+N58-N56</f>
-        <v>16590</v>
+        <v>3481</v>
       </c>
       <c r="O59" s="43" t="s">
         <v>84</v>
@@ -18349,7 +18349,7 @@
       <c r="M60"/>
       <c r="N60" s="92">
         <f>+N59/152.5%</f>
-        <v>10878.688524590165</v>
+        <v>2282.622950819672</v>
       </c>
       <c r="O60" s="43" t="s">
         <v>85</v>
@@ -18371,7 +18371,7 @@
       <c r="M61"/>
       <c r="N61" s="92">
         <f>+N60*52.5%</f>
-        <v>5711.3114754098369</v>
+        <v>1198.377049180328</v>
       </c>
       <c r="O61" s="43" t="s">
         <v>86</v>
@@ -18393,7 +18393,7 @@
       <c r="M62"/>
       <c r="N62" s="92">
         <f>+N60+N61</f>
-        <v>16590</v>
+        <v>3481</v>
       </c>
     </row>
     <row r="63" spans="1:18" ht="16" x14ac:dyDescent="0.2">

</xml_diff>